<commit_message>
Updated the model files
</commit_message>
<xml_diff>
--- a/model/makeSmallModel/reducedModel.xlsx
+++ b/model/makeSmallModel/reducedModel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="642">
   <si>
     <t>#</t>
   </si>
@@ -72,21 +72,24 @@
     <t>ENSG00000091140;ENSG00000110435;ENSG00000131828;ENSG00000150768;ENSG00000163114;ENSG00000168291</t>
   </si>
   <si>
+    <t>Tricarboxylic acid cycle</t>
+  </si>
+  <si>
+    <t>HMR_4388</t>
+  </si>
+  <si>
+    <t>H+[c] + NADH[c] + pyruvate[c] &lt;=&gt; L-lactate[c] + NAD+[c]</t>
+  </si>
+  <si>
+    <t>EC:1.1.1.27</t>
+  </si>
+  <si>
+    <t>ENSG00000111716;ENSG00000151116;ENSG00000166796;ENSG00000166800;ENSG00000171989;ENSG00000134333</t>
+  </si>
+  <si>
     <t>Glycolysis / Gluconeogenesis</t>
   </si>
   <si>
-    <t>HMR_4388</t>
-  </si>
-  <si>
-    <t>H+[c] + NADH[c] + pyruvate[c] &lt;=&gt; L-lactate[c] + NAD+[c]</t>
-  </si>
-  <si>
-    <t>EC:1.1.1.27</t>
-  </si>
-  <si>
-    <t>ENSG00000111716;ENSG00000151116;ENSG00000166796;ENSG00000166800;ENSG00000171989</t>
-  </si>
-  <si>
     <t>HMR_4379</t>
   </si>
   <si>
@@ -219,9 +222,6 @@
     <t>ENSG00000125166</t>
   </si>
   <si>
-    <t>Alanine, aspartate and glutamate metabolism</t>
-  </si>
-  <si>
     <t>HMR_3829</t>
   </si>
   <si>
@@ -243,9 +243,6 @@
     <t>ENSG00000067829;ENSG00000101365;ENSG00000166411</t>
   </si>
   <si>
-    <t>Tricarboxylic acid cycle and glyoxylate/dicarboxylate metabolism</t>
-  </si>
-  <si>
     <t>HMR_4139</t>
   </si>
   <si>
@@ -363,7 +360,7 @@
     <t>EC:3.6.1.3;EC:3.6.1.5;EC:3.6.3.1;EC:3.6.3.10;EC:3.6.3.14;EC:3.6.3.8;EC:3.6.3.9;EC:3.6.4.3;EC:3.6.4.4;EC:3.6.4.6;EC:3.6.4.12;EC:3.6.4.13</t>
   </si>
   <si>
-    <t>ENSG00000001626;ENSG00000004700;ENSG00000013573;ENSG00000017260;ENSG00000018625;ENSG00000021574;ENSG00000033627;ENSG00000039123;ENSG00000047249;ENSG00000054179;ENSG00000054793;ENSG00000058063;ENSG00000058668;ENSG00000064270;ENSG00000064703;ENSG00000067048;ENSG00000067596;ENSG00000067842;ENSG00000068650;ENSG00000069849;ENSG00000070961;ENSG00000071553;ENSG00000073111;ENSG00000073146;ENSG00000073969;ENSG00000074370;ENSG00000075673;ENSG00000076003;ENSG00000079785;ENSG00000080007;ENSG00000081923;ENSG00000085224;ENSG00000088205;ENSG00000089737;ENSG00000099624;ENSG00000100201;ENSG00000100297;ENSG00000100554;ENSG00000100888;ENSG00000101350;ENSG00000101452;ENSG00000101892;ENSG00000101974;ENSG00000102781;ENSG00000104043;ENSG00000104738;ENSG00000104884;ENSG00000105409;ENSG00000105671;ENSG00000105675;ENSG00000105929;ENSG00000107625;ENSG00000108469;ENSG00000108654;ENSG00000109606;ENSG00000110367;ENSG00000110719;ENSG00000110955;ENSG00000111364;ENSG00000111642;ENSG00000111877;ENSG00000112118;ENSG00000113732;ENSG00000114573;ENSG00000115267;ENSG00000116039;ENSG00000116254;ENSG00000116459;ENSG00000117410;ENSG00000118322;ENSG00000123136;ENSG00000123472;ENSG00000124172;ENSG00000124177;ENSG00000124228;ENSG00000124406;ENSG00000125375;ENSG00000125485;ENSG00000125885;ENSG00000127311;ENSG00000128524;ENSG00000128908;ENSG00000129244;ENSG00000130270;ENSG00000123064;ENSG00000131100;ENSG00000132153;ENSG00000132681;ENSG00000132932;ENSG00000134452;ENSG00000135390;ENSG00000135829;ENSG00000136271;ENSG00000136492;ENSG00000136888;ENSG00000138185;ENSG00000138346;ENSG00000138375;ENSG00000140451;ENSG00000140829;ENSG00000141141;ENSG00000141543;ENSG00000143153;ENSG00000143515;ENSG00000143882;ENSG00000144028;ENSG00000144045;ENSG00000145246;ENSG00000145833;ENSG00000147416;ENSG00000147614;ENSG00000150990;ENSG00000151418;ENSG00000152234;ENSG00000152670;ENSG00000153922;ENSG00000154518;ENSG00000154723;ENSG00000155097;ENSG00000156802;ENSG00000156976;ENSG00000157087;ENSG00000159199;ENSG00000159720;ENSG00000160957;ENSG00000162669;ENSG00000163104;ENSG00000163161;ENSG00000163214;ENSG00000163399;ENSG00000164080;ENSG00000165392;ENSG00000165629;ENSG00000165732;ENSG00000166377;ENSG00000166508;ENSG00000166833;ENSG00000167216;ENSG00000167283;ENSG00000167863;ENSG00000168032;ENSG00000169020;ENSG00000170004;ENSG00000171130;ENSG00000171302;ENSG00000171316;ENSG00000171953;ENSG00000173575;ENSG00000174243;ENSG00000174437;ENSG00000174953;ENSG00000177200;ENSG00000178105;ENSG00000183207;ENSG00000183258;ENSG00000185163;ENSG00000185344;ENSG00000185883;ENSG00000186009;ENSG00000186625;ENSG00000187240;ENSG00000188342;ENSG00000188833;ENSG00000196296;ENSG00000197299;ENSG00000198231;ENSG00000198563;ENSG00000198899;ENSG00000204560;ENSG00000206190;ENSG00000213760;ENSG00000213782;ENSG00000215301;ENSG00000229604;ENSG00000234920;ENSG00000241468;ENSG00000241837;ENSG00000249222;ENSG00000250565;ENSG00000258366</t>
+    <t>ENSG00000099624;ENSG00000110955;ENSG00000116459;ENSG00000124172;ENSG00000125375;ENSG00000135390;ENSG00000152234;ENSG00000154518;ENSG00000154723;ENSG00000159199;ENSG00000165629;ENSG00000167283;ENSG00000167863;ENSG00000169020;ENSG00000198899;ENSG00000241468;ENSG00000241837;ENSG00000123472;ENSG00000171953;ENSG00000229604;ENSG00000249222;ENSG00000228253;ENSG00000156411;ENSG00000173915</t>
   </si>
   <si>
     <t>HMR_6918</t>
@@ -375,7 +372,7 @@
     <t>EC:1.10.2.2</t>
   </si>
   <si>
-    <t>ENSG00000010256;ENSG00000127540;ENSG00000140740;ENSG00000156467;ENSG00000164405;ENSG00000169021;ENSG00000173660;ENSG00000179091;ENSG00000184076;ENSG00000198727</t>
+    <t>ENSG00000010256;ENSG00000127540;ENSG00000140740;ENSG00000156467;ENSG00000164405;ENSG00000169021;ENSG00000173660;ENSG00000179091;ENSG00000184076;ENSG00000198727;ENSG00000284493</t>
   </si>
   <si>
     <t>HMR_6921</t>
@@ -387,7 +384,7 @@
     <t>EC:1.6.5.3</t>
   </si>
   <si>
-    <t>ENSG00000004779;ENSG00000023228;ENSG00000065518;ENSG00000090266;ENSG00000099795;ENSG00000103356;ENSG00000109390;ENSG00000110717;ENSG00000113141;ENSG00000115286;ENSG00000119013;ENSG00000119421;ENSG00000125356;ENSG00000128609;ENSG00000130414;ENSG00000131495;ENSG00000136521;ENSG00000139180;ENSG00000140990;ENSG00000145494;ENSG00000147123;ENSG00000147684;ENSG00000151366;ENSG00000158864;ENSG00000160194;ENSG00000164258;ENSG00000165264;ENSG00000166136;ENSG00000167774;ENSG00000167792;ENSG00000168653;ENSG00000170906;ENSG00000174886;ENSG00000178127;ENSG00000183648;ENSG00000184752;ENSG00000184983;ENSG00000185633;ENSG00000186010;ENSG00000189043;ENSG00000198695;ENSG00000198763;ENSG00000198786;ENSG00000198840;ENSG00000198886;ENSG00000198888;ENSG00000212907;ENSG00000213619</t>
+    <t>ENSG00000004779;ENSG00000023228;ENSG00000065518;ENSG00000090266;ENSG00000099795;ENSG00000103356;ENSG00000109390;ENSG00000110717;ENSG00000113141;ENSG00000115286;ENSG00000119013;ENSG00000119421;ENSG00000125356;ENSG00000128609;ENSG00000130414;ENSG00000131495;ENSG00000136521;ENSG00000139180;ENSG00000140990;ENSG00000145494;ENSG00000147123;ENSG00000147684;ENSG00000151366;ENSG00000158864;ENSG00000160194;ENSG00000164258;ENSG00000165264;ENSG00000166136;ENSG00000167774;ENSG00000167792;ENSG00000168653;ENSG00000170906;ENSG00000174886;ENSG00000178127;ENSG00000183648;ENSG00000184752;ENSG00000184983;ENSG00000185633;ENSG00000186010;ENSG00000189043;ENSG00000198695;ENSG00000198763;ENSG00000198786;ENSG00000198840;ENSG00000198886;ENSG00000198888;ENSG00000212907;ENSG00000213619;ENSG00000283447</t>
   </si>
   <si>
     <t>HMR_0479</t>
@@ -591,6 +588,9 @@
     <t>Pi[c] + glycogen[c] =&gt; glucose-1-phosphate[c]</t>
   </si>
   <si>
+    <t>ENSG00000068976</t>
+  </si>
+  <si>
     <t>Starch and sucrose metabolism</t>
   </si>
   <si>
@@ -1305,12 +1305,6 @@
     <t>SHORT NAME</t>
   </si>
   <si>
-    <t>ENSG00000001626</t>
-  </si>
-  <si>
-    <t>ENSG00000004700</t>
-  </si>
-  <si>
     <t>ENSG00000004779</t>
   </si>
   <si>
@@ -1323,138 +1317,42 @@
     <t>ENSG00000010256</t>
   </si>
   <si>
-    <t>ENSG00000013573</t>
-  </si>
-  <si>
     <t>ENSG00000014641</t>
   </si>
   <si>
     <t>ENSG00000014919</t>
   </si>
   <si>
-    <t>ENSG00000017260</t>
-  </si>
-  <si>
-    <t>ENSG00000018625</t>
-  </si>
-  <si>
-    <t>ENSG00000021574</t>
-  </si>
-  <si>
     <t>ENSG00000023228</t>
   </si>
   <si>
-    <t>ENSG00000033627</t>
-  </si>
-  <si>
-    <t>ENSG00000039123</t>
-  </si>
-  <si>
-    <t>ENSG00000047249</t>
-  </si>
-  <si>
-    <t>ENSG00000054179</t>
-  </si>
-  <si>
-    <t>ENSG00000054793</t>
-  </si>
-  <si>
-    <t>ENSG00000058063</t>
-  </si>
-  <si>
-    <t>ENSG00000058668</t>
-  </si>
-  <si>
     <t>ENSG00000060762</t>
   </si>
   <si>
-    <t>ENSG00000064270</t>
-  </si>
-  <si>
-    <t>ENSG00000064703</t>
-  </si>
-  <si>
     <t>ENSG00000065518</t>
   </si>
   <si>
-    <t>ENSG00000067048</t>
-  </si>
-  <si>
     <t>ENSG00000067057</t>
   </si>
   <si>
     <t>ENSG00000067225</t>
   </si>
   <si>
-    <t>ENSG00000067596</t>
-  </si>
-  <si>
     <t>ENSG00000067829</t>
   </si>
   <si>
-    <t>ENSG00000067842</t>
-  </si>
-  <si>
-    <t>ENSG00000068650</t>
-  </si>
-  <si>
-    <t>ENSG00000069849</t>
-  </si>
-  <si>
-    <t>ENSG00000070961</t>
-  </si>
-  <si>
-    <t>ENSG00000071553</t>
-  </si>
-  <si>
-    <t>ENSG00000073111</t>
-  </si>
-  <si>
-    <t>ENSG00000073146</t>
-  </si>
-  <si>
     <t>ENSG00000073578</t>
   </si>
   <si>
-    <t>ENSG00000073969</t>
-  </si>
-  <si>
-    <t>ENSG00000074370</t>
-  </si>
-  <si>
     <t>ENSG00000074800</t>
   </si>
   <si>
-    <t>ENSG00000075673</t>
-  </si>
-  <si>
-    <t>ENSG00000076003</t>
-  </si>
-  <si>
     <t>ENSG00000079739</t>
   </si>
   <si>
-    <t>ENSG00000079785</t>
-  </si>
-  <si>
-    <t>ENSG00000080007</t>
-  </si>
-  <si>
-    <t>ENSG00000081923</t>
-  </si>
-  <si>
-    <t>ENSG00000085224</t>
-  </si>
-  <si>
     <t>ENSG00000086159</t>
   </si>
   <si>
-    <t>ENSG00000088205</t>
-  </si>
-  <si>
-    <t>ENSG00000089737</t>
-  </si>
-  <si>
     <t>ENSG00000090266</t>
   </si>
   <si>
@@ -1473,90 +1371,33 @@
     <t>ENSG00000100170</t>
   </si>
   <si>
-    <t>ENSG00000100201</t>
-  </si>
-  <si>
-    <t>ENSG00000100297</t>
-  </si>
-  <si>
     <t>ENSG00000100412</t>
   </si>
   <si>
-    <t>ENSG00000100554</t>
-  </si>
-  <si>
-    <t>ENSG00000100888</t>
-  </si>
-  <si>
-    <t>ENSG00000101350</t>
-  </si>
-  <si>
     <t>ENSG00000101365</t>
   </si>
   <si>
-    <t>ENSG00000101452</t>
-  </si>
-  <si>
-    <t>ENSG00000101892</t>
-  </si>
-  <si>
-    <t>ENSG00000101974</t>
-  </si>
-  <si>
     <t>ENSG00000102078</t>
   </si>
   <si>
     <t>ENSG00000102144</t>
   </si>
   <si>
-    <t>ENSG00000102781</t>
-  </si>
-  <si>
     <t>ENSG00000103356</t>
   </si>
   <si>
     <t>ENSG00000103375</t>
   </si>
   <si>
-    <t>ENSG00000104043</t>
-  </si>
-  <si>
-    <t>ENSG00000104738</t>
-  </si>
-  <si>
-    <t>ENSG00000104884</t>
-  </si>
-  <si>
-    <t>ENSG00000105409</t>
-  </si>
-  <si>
-    <t>ENSG00000105671</t>
-  </si>
-  <si>
-    <t>ENSG00000105675</t>
-  </si>
-  <si>
     <t>ENSG00000105679</t>
   </si>
   <si>
-    <t>ENSG00000105929</t>
-  </si>
-  <si>
     <t>ENSG00000105953</t>
   </si>
   <si>
-    <t>ENSG00000107625</t>
-  </si>
-  <si>
-    <t>ENSG00000108469</t>
-  </si>
-  <si>
     <t>ENSG00000108515</t>
   </si>
   <si>
-    <t>ENSG00000108654</t>
-  </si>
-  <si>
     <t>ENSG00000109107</t>
   </si>
   <si>
@@ -1566,33 +1407,18 @@
     <t>ENSG00000109424</t>
   </si>
   <si>
-    <t>ENSG00000109606</t>
-  </si>
-  <si>
-    <t>ENSG00000110367</t>
-  </si>
-  <si>
     <t>ENSG00000110435</t>
   </si>
   <si>
     <t>ENSG00000110717</t>
   </si>
   <si>
-    <t>ENSG00000110719</t>
-  </si>
-  <si>
     <t>ENSG00000110955</t>
   </si>
   <si>
-    <t>ENSG00000111364</t>
-  </si>
-  <si>
     <t>ENSG00000111640</t>
   </si>
   <si>
-    <t>ENSG00000111642</t>
-  </si>
-  <si>
     <t>ENSG00000111669</t>
   </si>
   <si>
@@ -1605,27 +1431,12 @@
     <t>ENSG00000111775</t>
   </si>
   <si>
-    <t>ENSG00000111877</t>
-  </si>
-  <si>
-    <t>ENSG00000112118</t>
-  </si>
-  <si>
     <t>ENSG00000112695</t>
   </si>
   <si>
     <t>ENSG00000113141</t>
   </si>
   <si>
-    <t>ENSG00000113732</t>
-  </si>
-  <si>
-    <t>ENSG00000114573</t>
-  </si>
-  <si>
-    <t>ENSG00000115267</t>
-  </si>
-  <si>
     <t>ENSG00000115286</t>
   </si>
   <si>
@@ -1635,24 +1446,12 @@
     <t>ENSG00000115944</t>
   </si>
   <si>
-    <t>ENSG00000116039</t>
-  </si>
-  <si>
-    <t>ENSG00000116254</t>
-  </si>
-  <si>
     <t>ENSG00000116459</t>
   </si>
   <si>
     <t>ENSG00000117118</t>
   </si>
   <si>
-    <t>ENSG00000117410</t>
-  </si>
-  <si>
-    <t>ENSG00000118322</t>
-  </si>
-  <si>
     <t>ENSG00000119013</t>
   </si>
   <si>
@@ -1671,75 +1470,36 @@
     <t>ENSG00000122729</t>
   </si>
   <si>
-    <t>ENSG00000123064</t>
-  </si>
-  <si>
-    <t>ENSG00000123136</t>
-  </si>
-  <si>
     <t>ENSG00000123472</t>
   </si>
   <si>
     <t>ENSG00000124172</t>
   </si>
   <si>
-    <t>ENSG00000124177</t>
-  </si>
-  <si>
-    <t>ENSG00000124228</t>
-  </si>
-  <si>
-    <t>ENSG00000124406</t>
-  </si>
-  <si>
     <t>ENSG00000125356</t>
   </si>
   <si>
     <t>ENSG00000125375</t>
   </si>
   <si>
-    <t>ENSG00000125485</t>
-  </si>
-  <si>
-    <t>ENSG00000125885</t>
-  </si>
-  <si>
     <t>ENSG00000126267</t>
   </si>
   <si>
     <t>ENSG00000127184</t>
   </si>
   <si>
-    <t>ENSG00000127311</t>
-  </si>
-  <si>
     <t>ENSG00000127540</t>
   </si>
   <si>
-    <t>ENSG00000128524</t>
-  </si>
-  <si>
     <t>ENSG00000128609</t>
   </si>
   <si>
-    <t>ENSG00000128908</t>
-  </si>
-  <si>
-    <t>ENSG00000129244</t>
-  </si>
-  <si>
-    <t>ENSG00000130270</t>
-  </si>
-  <si>
     <t>ENSG00000130414</t>
   </si>
   <si>
     <t>ENSG00000131055</t>
   </si>
   <si>
-    <t>ENSG00000131100</t>
-  </si>
-  <si>
     <t>ENSG00000131143</t>
   </si>
   <si>
@@ -1752,54 +1512,21 @@
     <t>ENSG00000131828</t>
   </si>
   <si>
-    <t>ENSG00000132153</t>
-  </si>
-  <si>
-    <t>ENSG00000132681</t>
-  </si>
-  <si>
-    <t>ENSG00000132932</t>
-  </si>
-  <si>
-    <t>ENSG00000134452</t>
-  </si>
-  <si>
     <t>ENSG00000135390</t>
   </si>
   <si>
-    <t>ENSG00000135829</t>
-  </si>
-  <si>
     <t>ENSG00000135940</t>
   </si>
   <si>
     <t>ENSG00000136143</t>
   </si>
   <si>
-    <t>ENSG00000136271</t>
-  </si>
-  <si>
-    <t>ENSG00000136492</t>
-  </si>
-  <si>
     <t>ENSG00000136521</t>
   </si>
   <si>
     <t>ENSG00000136872</t>
   </si>
   <si>
-    <t>ENSG00000136888</t>
-  </si>
-  <si>
-    <t>ENSG00000138185</t>
-  </si>
-  <si>
-    <t>ENSG00000138346</t>
-  </si>
-  <si>
-    <t>ENSG00000138375</t>
-  </si>
-  <si>
     <t>ENSG00000138400</t>
   </si>
   <si>
@@ -1809,39 +1536,21 @@
     <t>ENSG00000139180</t>
   </si>
   <si>
-    <t>ENSG00000140451</t>
-  </si>
-  <si>
     <t>ENSG00000140740</t>
   </si>
   <si>
-    <t>ENSG00000140829</t>
-  </si>
-  <si>
     <t>ENSG00000140990</t>
   </si>
   <si>
-    <t>ENSG00000141141</t>
-  </si>
-  <si>
-    <t>ENSG00000141543</t>
-  </si>
-  <si>
     <t>ENSG00000141959</t>
   </si>
   <si>
-    <t>ENSG00000143153</t>
-  </si>
-  <si>
     <t>ENSG00000143158</t>
   </si>
   <si>
     <t>ENSG00000143252</t>
   </si>
   <si>
-    <t>ENSG00000143515</t>
-  </si>
-  <si>
     <t>ENSG00000143595</t>
   </si>
   <si>
@@ -1851,33 +1560,12 @@
     <t>ENSG00000143630</t>
   </si>
   <si>
-    <t>ENSG00000143882</t>
-  </si>
-  <si>
-    <t>ENSG00000144028</t>
-  </si>
-  <si>
-    <t>ENSG00000144045</t>
-  </si>
-  <si>
-    <t>ENSG00000145246</t>
-  </si>
-  <si>
     <t>ENSG00000145494</t>
   </si>
   <si>
-    <t>ENSG00000145833</t>
-  </si>
-  <si>
     <t>ENSG00000147123</t>
   </si>
   <si>
-    <t>ENSG00000147416</t>
-  </si>
-  <si>
-    <t>ENSG00000147614</t>
-  </si>
-  <si>
     <t>ENSG00000147684</t>
   </si>
   <si>
@@ -1887,18 +1575,12 @@
     <t>ENSG00000150768</t>
   </si>
   <si>
-    <t>ENSG00000150990</t>
-  </si>
-  <si>
     <t>ENSG00000151116</t>
   </si>
   <si>
     <t>ENSG00000151366</t>
   </si>
   <si>
-    <t>ENSG00000151418</t>
-  </si>
-  <si>
     <t>ENSG00000151729</t>
   </si>
   <si>
@@ -1911,15 +1593,9 @@
     <t>ENSG00000152642</t>
   </si>
   <si>
-    <t>ENSG00000152670</t>
-  </si>
-  <si>
     <t>ENSG00000153291</t>
   </si>
   <si>
-    <t>ENSG00000153922</t>
-  </si>
-  <si>
     <t>ENSG00000154305</t>
   </si>
   <si>
@@ -1932,33 +1608,18 @@
     <t>ENSG00000154723</t>
   </si>
   <si>
-    <t>ENSG00000155097</t>
-  </si>
-  <si>
     <t>ENSG00000156467</t>
   </si>
   <si>
-    <t>ENSG00000156802</t>
-  </si>
-  <si>
     <t>ENSG00000156885</t>
   </si>
   <si>
-    <t>ENSG00000156976</t>
-  </si>
-  <si>
-    <t>ENSG00000157087</t>
-  </si>
-  <si>
     <t>ENSG00000158864</t>
   </si>
   <si>
     <t>ENSG00000159199</t>
   </si>
   <si>
-    <t>ENSG00000159720</t>
-  </si>
-  <si>
     <t>ENSG00000160194</t>
   </si>
   <si>
@@ -1968,39 +1629,18 @@
     <t>ENSG00000160471</t>
   </si>
   <si>
-    <t>ENSG00000160957</t>
-  </si>
-  <si>
     <t>ENSG00000161281</t>
   </si>
   <si>
     <t>ENSG00000161798</t>
   </si>
   <si>
-    <t>ENSG00000162669</t>
-  </si>
-  <si>
-    <t>ENSG00000163104</t>
-  </si>
-  <si>
     <t>ENSG00000163114</t>
   </si>
   <si>
-    <t>ENSG00000163161</t>
-  </si>
-  <si>
-    <t>ENSG00000163214</t>
-  </si>
-  <si>
-    <t>ENSG00000163399</t>
-  </si>
-  <si>
     <t>ENSG00000163541</t>
   </si>
   <si>
-    <t>ENSG00000164080</t>
-  </si>
-  <si>
     <t>ENSG00000164258</t>
   </si>
   <si>
@@ -2022,39 +1662,21 @@
     <t>ENSG00000165272</t>
   </si>
   <si>
-    <t>ENSG00000165392</t>
-  </si>
-  <si>
     <t>ENSG00000165629</t>
   </si>
   <si>
-    <t>ENSG00000165732</t>
-  </si>
-  <si>
     <t>ENSG00000166136</t>
   </si>
   <si>
-    <t>ENSG00000166377</t>
-  </si>
-  <si>
     <t>ENSG00000166411</t>
   </si>
   <si>
-    <t>ENSG00000166508</t>
-  </si>
-  <si>
     <t>ENSG00000166796</t>
   </si>
   <si>
     <t>ENSG00000166800</t>
   </si>
   <si>
-    <t>ENSG00000166833</t>
-  </si>
-  <si>
-    <t>ENSG00000167216</t>
-  </si>
-  <si>
     <t>ENSG00000167283</t>
   </si>
   <si>
@@ -2073,9 +1695,6 @@
     <t>ENSG00000167863</t>
   </si>
   <si>
-    <t>ENSG00000168032</t>
-  </si>
-  <si>
     <t>ENSG00000168291</t>
   </si>
   <si>
@@ -2097,9 +1716,6 @@
     <t>ENSG00000169299</t>
   </si>
   <si>
-    <t>ENSG00000170004</t>
-  </si>
-  <si>
     <t>ENSG00000170516</t>
   </si>
   <si>
@@ -2109,18 +1725,9 @@
     <t>ENSG00000170950</t>
   </si>
   <si>
-    <t>ENSG00000171130</t>
-  </si>
-  <si>
-    <t>ENSG00000171302</t>
-  </si>
-  <si>
     <t>ENSG00000171314</t>
   </si>
   <si>
-    <t>ENSG00000171316</t>
-  </si>
-  <si>
     <t>ENSG00000171885</t>
   </si>
   <si>
@@ -2136,24 +1743,12 @@
     <t>ENSG00000172340</t>
   </si>
   <si>
-    <t>ENSG00000173575</t>
-  </si>
-  <si>
     <t>ENSG00000173660</t>
   </si>
   <si>
-    <t>ENSG00000174243</t>
-  </si>
-  <si>
-    <t>ENSG00000174437</t>
-  </si>
-  <si>
     <t>ENSG00000174886</t>
   </si>
   <si>
-    <t>ENSG00000174953</t>
-  </si>
-  <si>
     <t>ENSG00000175564</t>
   </si>
   <si>
@@ -2163,12 +1758,6 @@
     <t>ENSG00000176340</t>
   </si>
   <si>
-    <t>ENSG00000177200</t>
-  </si>
-  <si>
-    <t>ENSG00000178105</t>
-  </si>
-  <si>
     <t>ENSG00000178127</t>
   </si>
   <si>
@@ -2184,12 +1773,6 @@
     <t>ENSG00000181192</t>
   </si>
   <si>
-    <t>ENSG00000183207</t>
-  </si>
-  <si>
-    <t>ENSG00000183258</t>
-  </si>
-  <si>
     <t>ENSG00000183648</t>
   </si>
   <si>
@@ -2202,57 +1785,21 @@
     <t>ENSG00000184983</t>
   </si>
   <si>
-    <t>ENSG00000185163</t>
-  </si>
-  <si>
-    <t>ENSG00000185344</t>
-  </si>
-  <si>
     <t>ENSG00000185633</t>
   </si>
   <si>
-    <t>ENSG00000185883</t>
-  </si>
-  <si>
-    <t>ENSG00000186009</t>
-  </si>
-  <si>
     <t>ENSG00000186010</t>
   </si>
   <si>
-    <t>ENSG00000186625</t>
-  </si>
-  <si>
-    <t>ENSG00000187240</t>
-  </si>
-  <si>
     <t>ENSG00000187581</t>
   </si>
   <si>
-    <t>ENSG00000188342</t>
-  </si>
-  <si>
-    <t>ENSG00000188833</t>
-  </si>
-  <si>
     <t>ENSG00000189043</t>
   </si>
   <si>
-    <t>ENSG00000196296</t>
-  </si>
-  <si>
-    <t>ENSG00000197299</t>
-  </si>
-  <si>
     <t>ENSG00000197444</t>
   </si>
   <si>
-    <t>ENSG00000198231</t>
-  </si>
-  <si>
-    <t>ENSG00000198563</t>
-  </si>
-  <si>
     <t>ENSG00000198695</t>
   </si>
   <si>
@@ -2289,27 +1836,12 @@
     <t>ENSG00000204370</t>
   </si>
   <si>
-    <t>ENSG00000204560</t>
-  </si>
-  <si>
-    <t>ENSG00000206190</t>
-  </si>
-  <si>
     <t>ENSG00000212907</t>
   </si>
   <si>
     <t>ENSG00000213619</t>
   </si>
   <si>
-    <t>ENSG00000213760</t>
-  </si>
-  <si>
-    <t>ENSG00000213782</t>
-  </si>
-  <si>
-    <t>ENSG00000215301</t>
-  </si>
-  <si>
     <t>ENSG00000226784</t>
   </si>
   <si>
@@ -2319,9 +1851,6 @@
     <t>ENSG00000230359</t>
   </si>
   <si>
-    <t>ENSG00000234920</t>
-  </si>
-  <si>
     <t>ENSG00000235957</t>
   </si>
   <si>
@@ -2343,19 +1872,28 @@
     <t>ENSG00000249222</t>
   </si>
   <si>
-    <t>ENSG00000250565</t>
-  </si>
-  <si>
     <t>ENSG00000250630</t>
   </si>
   <si>
-    <t>ENSG00000258366</t>
-  </si>
-  <si>
     <t>DLSTP1</t>
   </si>
   <si>
     <t>LOC642502</t>
+  </si>
+  <si>
+    <t>ENSG00000283447</t>
+  </si>
+  <si>
+    <t>ENSG00000284493</t>
+  </si>
+  <si>
+    <t>ENSG00000228253</t>
+  </si>
+  <si>
+    <t>ENSG00000156411</t>
+  </si>
+  <si>
+    <t>ENSG00000173915</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -2532,227 +2070,227 @@
         <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L12" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
@@ -2766,13 +2304,13 @@
         <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
         <v>70</v>
       </c>
       <c r="L15" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -2792,322 +2330,322 @@
         <v>74</v>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>76</v>
       </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>77</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>78</v>
       </c>
-      <c r="F17" t="s">
-        <v>79</v>
-      </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>80</v>
       </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
         <v>81</v>
       </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" t="s">
-        <v>82</v>
-      </c>
       <c r="L18" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>84</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>85</v>
       </c>
-      <c r="F19" t="s">
-        <v>86</v>
-      </c>
       <c r="L19" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>89</v>
       </c>
-      <c r="F20" t="s">
-        <v>90</v>
-      </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
         <v>91</v>
       </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>93</v>
       </c>
-      <c r="F21" t="s">
-        <v>94</v>
-      </c>
       <c r="L21" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
         <v>95</v>
       </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>96</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>97</v>
       </c>
-      <c r="F22" t="s">
-        <v>98</v>
-      </c>
       <c r="L22" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
         <v>99</v>
       </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>101</v>
       </c>
-      <c r="F23" t="s">
-        <v>102</v>
-      </c>
       <c r="L23" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
         <v>103</v>
       </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>105</v>
       </c>
-      <c r="F24" t="s">
-        <v>106</v>
-      </c>
       <c r="L24" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
         <v>107</v>
       </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>108</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>109</v>
       </c>
-      <c r="F25" t="s">
+      <c r="L25" t="s">
         <v>110</v>
-      </c>
-      <c r="L25" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
         <v>112</v>
       </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>113</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>114</v>
       </c>
-      <c r="F26" t="s">
-        <v>115</v>
-      </c>
       <c r="L26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
         <v>116</v>
       </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>117</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>118</v>
       </c>
-      <c r="F27" t="s">
-        <v>119</v>
-      </c>
       <c r="L27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
         <v>120</v>
       </c>
-      <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>121</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>122</v>
       </c>
-      <c r="F28" t="s">
-        <v>123</v>
-      </c>
       <c r="L28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
         <v>124</v>
       </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>125</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>126</v>
       </c>
-      <c r="F29" t="s">
+      <c r="L29" t="s">
         <v>127</v>
-      </c>
-      <c r="L29" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
         <v>129</v>
       </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>130</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>131</v>
-      </c>
-      <c r="F30" t="s">
-        <v>132</v>
       </c>
       <c r="G30" t="n">
         <v>-1000.0</v>
       </c>
       <c r="L30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
         <v>133</v>
       </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
         <v>134</v>
       </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="L31" t="s">
         <v>135</v>
-      </c>
-      <c r="L31" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
         <v>137</v>
       </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" t="s">
-        <v>138</v>
-      </c>
       <c r="E32" t="s">
         <v>14</v>
       </c>
@@ -3115,19 +2653,19 @@
         <v>14</v>
       </c>
       <c r="L32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
         <v>139</v>
       </c>
-      <c r="C33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" t="s">
-        <v>140</v>
-      </c>
       <c r="E33" t="s">
         <v>14</v>
       </c>
@@ -3135,19 +2673,19 @@
         <v>14</v>
       </c>
       <c r="L33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
         <v>141</v>
       </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s">
-        <v>142</v>
-      </c>
       <c r="E34" t="s">
         <v>14</v>
       </c>
@@ -3155,39 +2693,39 @@
         <v>14</v>
       </c>
       <c r="L34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
         <v>143</v>
       </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>144</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>145</v>
       </c>
-      <c r="F35" t="s">
+      <c r="L35" t="s">
         <v>146</v>
-      </c>
-      <c r="L35" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
         <v>148</v>
       </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" t="s">
-        <v>149</v>
-      </c>
       <c r="E36" t="s">
         <v>14</v>
       </c>
@@ -3195,39 +2733,39 @@
         <v>14</v>
       </c>
       <c r="L36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
         <v>150</v>
       </c>
-      <c r="C37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>151</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>152</v>
       </c>
-      <c r="F37" t="s">
-        <v>153</v>
-      </c>
       <c r="L37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
         <v>154</v>
       </c>
-      <c r="C38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" t="s">
-        <v>155</v>
-      </c>
       <c r="E38" t="s">
         <v>14</v>
       </c>
@@ -3235,19 +2773,19 @@
         <v>14</v>
       </c>
       <c r="L38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
         <v>156</v>
       </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" t="s">
-        <v>157</v>
-      </c>
       <c r="E39" t="s">
         <v>14</v>
       </c>
@@ -3255,19 +2793,19 @@
         <v>14</v>
       </c>
       <c r="L39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
         <v>158</v>
       </c>
-      <c r="C40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" t="s">
-        <v>159</v>
-      </c>
       <c r="E40" t="s">
         <v>14</v>
       </c>
@@ -3275,118 +2813,118 @@
         <v>14</v>
       </c>
       <c r="L40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
         <v>160</v>
       </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
         <v>161</v>
       </c>
-      <c r="E41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" t="s">
-        <v>162</v>
-      </c>
       <c r="L41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
         <v>163</v>
       </c>
-      <c r="C42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>164</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>165</v>
       </c>
-      <c r="F42" t="s">
-        <v>166</v>
-      </c>
       <c r="L42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
         <v>167</v>
       </c>
-      <c r="C43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" t="s">
         <v>168</v>
       </c>
-      <c r="E43" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" t="s">
-        <v>169</v>
-      </c>
       <c r="L43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
         <v>170</v>
       </c>
-      <c r="C44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" t="s">
         <v>171</v>
       </c>
-      <c r="E44" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" t="s">
-        <v>172</v>
-      </c>
       <c r="L44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
         <v>173</v>
       </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+      <c r="L45" t="s">
         <v>174</v>
-      </c>
-      <c r="E45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" t="s">
-        <v>14</v>
-      </c>
-      <c r="L45" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
         <v>176</v>
-      </c>
-      <c r="C46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" t="s">
-        <v>177</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
@@ -3401,19 +2939,19 @@
         <v>0.0</v>
       </c>
       <c r="L46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
         <v>178</v>
       </c>
-      <c r="C47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" t="s">
-        <v>179</v>
-      </c>
       <c r="E47" t="s">
         <v>14</v>
       </c>
@@ -3421,18 +2959,18 @@
         <v>14</v>
       </c>
       <c r="L47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
         <v>180</v>
-      </c>
-      <c r="C48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" t="s">
-        <v>181</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
@@ -3444,18 +2982,18 @@
         <v>0.0</v>
       </c>
       <c r="L48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
         <v>182</v>
-      </c>
-      <c r="C49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" t="s">
-        <v>183</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -3470,18 +3008,18 @@
         <v>0.0</v>
       </c>
       <c r="L49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
         <v>184</v>
-      </c>
-      <c r="C50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" t="s">
-        <v>185</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -3493,19 +3031,19 @@
         <v>1.0</v>
       </c>
       <c r="L50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s">
         <v>187</v>
       </c>
-      <c r="C51" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" t="s">
-        <v>188</v>
-      </c>
       <c r="E51" t="s">
         <v>14</v>
       </c>
@@ -3513,24 +3051,24 @@
         <v>14</v>
       </c>
       <c r="L51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
         <v>189</v>
       </c>
-      <c r="C52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="s">
         <v>190</v>
-      </c>
-      <c r="E52" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52" t="s">
-        <v>14</v>
       </c>
       <c r="L52" t="s">
         <v>191</v>
@@ -5070,942 +4608,942 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>437</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>444</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>449</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>86</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>459</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>463</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>166</v>
+        <v>465</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>476</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>477</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>489</v>
+        <v>67</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>54</v>
+        <v>499</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>153</v>
+        <v>509</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>517</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>132</v>
+        <v>532</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>66</v>
+        <v>556</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="178">
       <c r="B178" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="179">
       <c r="B179" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="180">
       <c r="B180" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="187">
       <c r="B187" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="188">
       <c r="B188" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="189">
       <c r="B189" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="190">
       <c r="B190" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="191">
       <c r="B191" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="192">
       <c r="B192" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="193">
       <c r="B193" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="194">
       <c r="B194" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="195">
       <c r="B195" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="196">
       <c r="B196" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="197">
       <c r="B197" t="s">
-        <v>82</v>
+        <v>616</v>
       </c>
     </row>
     <row r="198">
@@ -6051,776 +5589,6 @@
     <row r="206">
       <c r="B206" t="s">
         <v>625</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="B207" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="B208" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="B209" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="B210" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="B211" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="B212" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="B213" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="B214" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="B215" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="B216" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="B217" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="B218" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="B219" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="B220" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="B221" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="B222" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="B223" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="B224" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="B225" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="B226" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="B227" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="B228" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="B229" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="B230" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="B231" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="B232" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="B233" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="B234" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="B235" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="B236" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="B237" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="B238" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="B239" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="B240" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="B241" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="B242" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="B243" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="B244" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="B245" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="B246" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="B247" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="B248" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="B249" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="B250" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="B251" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="B252" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="B253" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="B254" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="B255" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="B256" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="B257" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="B258" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="B259" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="B260" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="B261" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="B262" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="B263" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="B264" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="B265" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="B266" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="B267" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="B268" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="B269" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="B270" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="B271" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="B272" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="B273" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="B274" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="B275" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="B276" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="B277" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="B278" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="B279" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="B280" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="B281" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="B282" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="B283" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="B284" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="B285" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="B286" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="B287" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="B288" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="B289" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="B290" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="291">
-      <c r="B291" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="292">
-      <c r="B292" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="293">
-      <c r="B293" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="294">
-      <c r="B294" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="295">
-      <c r="B295" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="296">
-      <c r="B296" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="297">
-      <c r="B297" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="298">
-      <c r="B298" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="299">
-      <c r="B299" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="300">
-      <c r="B300" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="301">
-      <c r="B301" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="302">
-      <c r="B302" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="303">
-      <c r="B303" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="304">
-      <c r="B304" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="305">
-      <c r="B305" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="306">
-      <c r="B306" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="307">
-      <c r="B307" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="308">
-      <c r="B308" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="309">
-      <c r="B309" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="310">
-      <c r="B310" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="311">
-      <c r="B311" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="312">
-      <c r="B312" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="313">
-      <c r="B313" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="314">
-      <c r="B314" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="315">
-      <c r="B315" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="316">
-      <c r="B316" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="317">
-      <c r="B317" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="318">
-      <c r="B318" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="B319" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="B320" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="B321" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="322">
-      <c r="B322" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="323">
-      <c r="B323" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="324">
-      <c r="B324" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="325">
-      <c r="B325" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="326">
-      <c r="B326" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="327">
-      <c r="B327" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="328">
-      <c r="B328" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="329">
-      <c r="B329" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="330">
-      <c r="B330" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="B331" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="B332" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="B333" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="B334" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="B335" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="B336" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="B337" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="B338" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="B339" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="B340" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="B341" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="B342" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="B343" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="B344" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="B345" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="B346" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="B347" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="B348" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="B349" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="B350" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="B351" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="B352" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="B353" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="B354" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="B355" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="B356" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="B357" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="B358" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="B359" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="B360" t="s">
-        <v>779</v>
       </c>
     </row>
   </sheetData>
@@ -6844,39 +5612,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>780</v>
+        <v>626</v>
       </c>
       <c r="D1" t="s">
-        <v>781</v>
+        <v>627</v>
       </c>
       <c r="E1" t="s">
-        <v>782</v>
+        <v>628</v>
       </c>
       <c r="F1" t="s">
-        <v>783</v>
+        <v>629</v>
       </c>
       <c r="G1" t="s">
-        <v>784</v>
+        <v>630</v>
       </c>
       <c r="H1" t="s">
-        <v>785</v>
+        <v>631</v>
       </c>
       <c r="I1" t="s">
-        <v>786</v>
+        <v>632</v>
       </c>
       <c r="J1" t="s">
-        <v>787</v>
+        <v>633</v>
       </c>
       <c r="K1" t="s">
-        <v>788</v>
+        <v>634</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>789</v>
+        <v>635</v>
       </c>
       <c r="C2" t="s">
-        <v>790</v>
+        <v>636</v>
       </c>
       <c r="D2" t="n">
         <v>-1000.0</v>
@@ -6885,19 +5653,19 @@
         <v>1000.0</v>
       </c>
       <c r="F2" t="s">
-        <v>791</v>
+        <v>637</v>
       </c>
       <c r="G2" t="s">
-        <v>792</v>
+        <v>638</v>
       </c>
       <c r="H2" t="s">
-        <v>793</v>
+        <v>639</v>
       </c>
       <c r="I2" t="s">
-        <v>794</v>
+        <v>640</v>
       </c>
       <c r="J2" t="s">
-        <v>795</v>
+        <v>641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>